<commit_message>
update 2022-3 and add 2022-4
</commit_message>
<xml_diff>
--- a/source/_posts/collection/new-words.xlsx
+++ b/source/_posts/collection/new-words.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuxiyang/myData/python-project/liuxiyang641.github.io/source/_posts/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F659F9-79A7-7042-AEEE-81FAE84A1373}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E817BC9F-3822-0645-AD30-88E9D02ADB7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="-21140" windowWidth="33600" windowHeight="20540" xr2:uid="{C07A63B5-5344-AF4A-AFD6-2139CC657E22}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="663">
   <si>
     <t>[rɪˈtriːvl]</t>
   </si>
@@ -3343,6 +3343,78 @@
   </si>
   <si>
     <t xml:space="preserve"> /riː'kɑːst/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>intriguing</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Aside from being an </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>intriguing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> theoretical question, the size-generalization problem has important practical implications.</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>readily</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>容易的，没有难度的</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">It can be </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>readily</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> seen that when training the model on graphs where the ratio n/m between the number of nodes and number of edges is ﬁxed, gradient descent with a small enough learning rate will favor the global solution</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> /'redɪlɪ/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/ɪnˈtri:gɪŋ/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>有趣的，引入入胜的</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3832,7 +3904,7 @@
   <dimension ref="A1:H696"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A258" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F269" sqref="F269"/>
+      <selection activeCell="E265" sqref="E265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -7328,21 +7400,39 @@
         <v>652</v>
       </c>
     </row>
-    <row r="265" spans="1:5">
+    <row r="265" spans="1:5" ht="57">
       <c r="A265" s="18">
         <v>264</v>
       </c>
-      <c r="B265" s="3"/>
-      <c r="C265" s="3"/>
-      <c r="D265" s="12"/>
-    </row>
-    <row r="266" spans="1:5">
+      <c r="B265" s="3" t="s">
+        <v>655</v>
+      </c>
+      <c r="C265" s="3" t="s">
+        <v>661</v>
+      </c>
+      <c r="D265" s="12" t="s">
+        <v>662</v>
+      </c>
+      <c r="E265" s="17" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" ht="114">
       <c r="A266" s="18">
         <v>265</v>
       </c>
-      <c r="B266" s="3"/>
-      <c r="C266" s="3"/>
-      <c r="D266" s="12"/>
+      <c r="B266" s="3" t="s">
+        <v>657</v>
+      </c>
+      <c r="C266" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="D266" s="12" t="s">
+        <v>658</v>
+      </c>
+      <c r="E266" s="17" t="s">
+        <v>659</v>
+      </c>
     </row>
     <row r="267" spans="1:5">
       <c r="A267" s="18">

</xml_diff>

<commit_message>
update 2022-5 and GPT-1
</commit_message>
<xml_diff>
--- a/source/_posts/collection/new-words.xlsx
+++ b/source/_posts/collection/new-words.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuxiyang/myData/python-project/liuxiyang641.github.io/source/_posts/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E817BC9F-3822-0645-AD30-88E9D02ADB7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7737C77D-B980-634B-9C72-EC0158AB98BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="-21140" windowWidth="33600" windowHeight="20540" xr2:uid="{C07A63B5-5344-AF4A-AFD6-2139CC657E22}"/>
+    <workbookView xWindow="47780" yWindow="-21040" windowWidth="33600" windowHeight="20540" xr2:uid="{C07A63B5-5344-AF4A-AFD6-2139CC657E22}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,12 +23,20 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="674">
   <si>
     <t>[rɪˈtriːvl]</t>
   </si>
@@ -241,9 +249,6 @@
   </si>
   <si>
     <t>剩余的，残留的</t>
-  </si>
-  <si>
-    <t>leverage</t>
   </si>
   <si>
     <t>影响，利用</t>
@@ -3415,6 +3420,135 @@
   </si>
   <si>
     <t>有趣的，引入入胜的</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>leverage</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>dearth</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>缺乏</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Most deep learning methods require substantial amounts of manually labeled data, which restricts their applicability in many domains that suffer from </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>a dearth of</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> annotated resources.</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>/dɜːθ/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>compelling</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> /kəmˈpelɪŋ/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>令人信服的，有说服力的；有吸引力的</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The most </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>compelling</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> evidence for this so far has been the extensive use of pretrained word embeddings [10, 39, 42] to improve performance on a range of NLP tasks.</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This is </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>in line with</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> prior work [50, 43], who also observed improved performance with such an auxiliary objective.</t>
+    </r>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>is in line with</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>符合；保持一致（可以用来替换</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>following</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="SimSun"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>）</t>
+    </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -3903,8 +4037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B4733E-376B-124B-AFDB-49936A421CEF}">
   <dimension ref="A1:H696"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A258" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E265" sqref="E265"/>
+    <sheetView tabSelected="1" topLeftCell="A266" zoomScale="125" workbookViewId="0">
+      <selection activeCell="D274" sqref="D274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -3929,7 +4063,7 @@
         <v>8</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="19">
@@ -4266,13 +4400,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>662</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26" s="12" t="s">
         <v>71</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" s="12" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="19">
@@ -4280,11 +4414,11 @@
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="19">
@@ -4292,13 +4426,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="D28" s="12" t="s">
         <v>77</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="19">
@@ -4306,11 +4440,11 @@
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="12" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="19">
@@ -4318,13 +4452,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="D30" s="12" t="s">
         <v>82</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="19">
@@ -4332,13 +4466,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="12" t="s">
         <v>84</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="19">
@@ -4346,13 +4480,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D32" s="12" t="s">
         <v>87</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="19">
@@ -4360,11 +4494,11 @@
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="19">
@@ -4372,11 +4506,11 @@
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="19">
@@ -4384,13 +4518,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="D35" s="12" t="s">
         <v>95</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="19">
@@ -4398,13 +4532,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36" s="12" t="s">
         <v>97</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="19">
@@ -4412,13 +4546,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37" s="12" t="s">
         <v>100</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="19">
@@ -4426,11 +4560,11 @@
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="19">
@@ -4438,13 +4572,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="D39" s="12" t="s">
         <v>106</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="19">
@@ -4452,13 +4586,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D40" s="12" t="s">
         <v>109</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="19">
@@ -4466,13 +4600,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="38">
@@ -4480,11 +4614,11 @@
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="19">
@@ -4492,11 +4626,11 @@
         <v>42</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="19">
@@ -4504,11 +4638,11 @@
         <v>43</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="57">
@@ -4516,11 +4650,11 @@
         <v>44</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="19">
@@ -4528,13 +4662,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D46" s="14" t="s">
         <v>121</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="38">
@@ -4542,11 +4676,11 @@
         <v>46</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C47" s="4"/>
       <c r="D47" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="19">
@@ -4554,11 +4688,11 @@
         <v>47</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="20">
@@ -4566,13 +4700,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="19">
@@ -4580,13 +4714,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D50" s="12" t="s">
         <v>130</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D50" s="12" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="19">
@@ -4594,10 +4728,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="D51" s="12"/>
     </row>
@@ -4606,13 +4740,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D52" s="12" t="s">
         <v>135</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="19">
@@ -4620,11 +4754,11 @@
         <v>52</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="19">
@@ -4632,13 +4766,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C54" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="D54" s="12" t="s">
         <v>141</v>
-      </c>
-      <c r="D54" s="12" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="19">
@@ -4646,13 +4780,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="D55" s="12" t="s">
         <v>144</v>
-      </c>
-      <c r="D55" s="12" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="19">
@@ -4660,11 +4794,11 @@
         <v>55</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="19">
@@ -4672,11 +4806,11 @@
         <v>56</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C57" s="3"/>
       <c r="D57" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="19">
@@ -4684,11 +4818,11 @@
         <v>57</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C58" s="3"/>
       <c r="D58" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="19">
@@ -4696,11 +4830,11 @@
         <v>58</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="19">
@@ -4708,11 +4842,11 @@
         <v>59</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="12" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="19">
@@ -4720,11 +4854,11 @@
         <v>60</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="19">
@@ -4732,11 +4866,11 @@
         <v>61</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C62" s="3"/>
       <c r="D62" s="12" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="19">
@@ -4744,11 +4878,11 @@
         <v>62</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="12" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="19">
@@ -4756,11 +4890,11 @@
         <v>63</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="19">
@@ -4768,13 +4902,13 @@
         <v>64</v>
       </c>
       <c r="B65" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D65" s="12" t="s">
         <v>164</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="D65" s="12" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="19">
@@ -4782,11 +4916,11 @@
         <v>65</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C66" s="3"/>
       <c r="D66" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="20">
@@ -4794,13 +4928,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="C67" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="D67" s="12" t="s">
         <v>170</v>
-      </c>
-      <c r="D67" s="12" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="19">
@@ -4808,11 +4942,11 @@
         <v>67</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C68" s="3"/>
       <c r="D68" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="19">
@@ -4820,13 +4954,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="D69" s="12" t="s">
         <v>175</v>
-      </c>
-      <c r="D69" s="12" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="19">
@@ -4834,13 +4968,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="D70" s="12" t="s">
         <v>177</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D70" s="12" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="19">
@@ -4848,11 +4982,11 @@
         <v>70</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C71" s="3"/>
       <c r="D71" s="12" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="19">
@@ -4860,11 +4994,11 @@
         <v>71</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C72" s="3"/>
       <c r="D72" s="12" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="19">
@@ -4872,11 +5006,11 @@
         <v>72</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="12" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="19">
@@ -4884,11 +5018,11 @@
         <v>73</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C74" s="3"/>
       <c r="D74" s="12" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="19">
@@ -4896,13 +5030,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D75" s="12" t="s">
         <v>188</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="D75" s="12" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="19">
@@ -4910,11 +5044,11 @@
         <v>75</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="19">
@@ -4922,11 +5056,11 @@
         <v>76</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="12" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="19">
@@ -4934,13 +5068,13 @@
         <v>77</v>
       </c>
       <c r="B78" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D78" s="12" t="s">
         <v>195</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="D78" s="12" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="19">
@@ -4948,11 +5082,11 @@
         <v>78</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="12" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="19">
@@ -4960,11 +5094,11 @@
         <v>79</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="19">
@@ -4972,11 +5106,11 @@
         <v>80</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C81" s="3"/>
       <c r="D81" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="19">
@@ -4984,11 +5118,11 @@
         <v>81</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C82" s="3"/>
       <c r="D82" s="12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="19">
@@ -4996,11 +5130,11 @@
         <v>82</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C83" s="3"/>
       <c r="D83" s="12" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="19">
@@ -5008,11 +5142,11 @@
         <v>83</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C84" s="3"/>
       <c r="D84" s="13" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="20">
@@ -5020,13 +5154,13 @@
         <v>84</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D85" s="12" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="19">
@@ -5034,13 +5168,13 @@
         <v>85</v>
       </c>
       <c r="B86" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C86" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="C86" s="3" t="s">
+      <c r="D86" s="12" t="s">
         <v>213</v>
-      </c>
-      <c r="D86" s="12" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="19">
@@ -5048,11 +5182,11 @@
         <v>86</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C87" s="3"/>
       <c r="D87" s="12" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="36">
@@ -5060,13 +5194,13 @@
         <v>87</v>
       </c>
       <c r="B88" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C88" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="C88" s="3" t="s">
-        <v>218</v>
-      </c>
       <c r="D88" s="12" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="19">
@@ -5074,11 +5208,11 @@
         <v>88</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C89" s="3"/>
       <c r="D89" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="19">
@@ -5086,11 +5220,11 @@
         <v>89</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C90" s="3"/>
       <c r="D90" s="12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="20">
@@ -5098,13 +5232,13 @@
         <v>90</v>
       </c>
       <c r="B91" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C91" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="C91" s="3" t="s">
+      <c r="D91" s="12" t="s">
         <v>224</v>
-      </c>
-      <c r="D91" s="12" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="19">
@@ -5112,11 +5246,11 @@
         <v>91</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C92" s="3"/>
       <c r="D92" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="20">
@@ -5124,13 +5258,13 @@
         <v>92</v>
       </c>
       <c r="B93" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C93" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="C93" s="3" t="s">
+      <c r="D93" s="12" t="s">
         <v>230</v>
-      </c>
-      <c r="D93" s="12" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="19">
@@ -5138,11 +5272,11 @@
         <v>93</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C94" s="3"/>
       <c r="D94" s="13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="19">
@@ -5150,13 +5284,13 @@
         <v>94</v>
       </c>
       <c r="B95" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C95" s="3" t="s">
         <v>234</v>
       </c>
-      <c r="C95" s="3" t="s">
+      <c r="D95" s="13" t="s">
         <v>235</v>
-      </c>
-      <c r="D95" s="13" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="19">
@@ -5164,11 +5298,11 @@
         <v>95</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C96" s="3"/>
       <c r="D96" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="20">
@@ -5176,13 +5310,13 @@
         <v>96</v>
       </c>
       <c r="B97" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="C97" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="C97" s="3" t="s">
+      <c r="D97" s="12" t="s">
         <v>240</v>
-      </c>
-      <c r="D97" s="12" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="20">
@@ -5190,13 +5324,13 @@
         <v>97</v>
       </c>
       <c r="B98" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C98" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="C98" s="3" t="s">
+      <c r="D98" s="12" t="s">
         <v>243</v>
-      </c>
-      <c r="D98" s="12" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="19">
@@ -5204,11 +5338,11 @@
         <v>98</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C99" s="3"/>
       <c r="D99" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="38">
@@ -5216,7 +5350,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C100" s="3"/>
       <c r="D100" s="12"/>
@@ -5226,11 +5360,11 @@
         <v>100</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C101" s="3"/>
       <c r="D101" s="12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="19">
@@ -5238,13 +5372,13 @@
         <v>101</v>
       </c>
       <c r="B102" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="D102" s="12" t="s">
         <v>250</v>
-      </c>
-      <c r="C102" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="D102" s="12" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="19">
@@ -5252,7 +5386,7 @@
         <v>102</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C103" s="3"/>
       <c r="D103" s="12"/>
@@ -5262,11 +5396,11 @@
         <v>103</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="12" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="19">
@@ -5274,11 +5408,11 @@
         <v>104</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C105" s="3"/>
       <c r="D105" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -5286,13 +5420,13 @@
         <v>105</v>
       </c>
       <c r="B106" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="C106" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="C106" s="4" t="s">
+      <c r="D106" s="10" t="s">
         <v>259</v>
-      </c>
-      <c r="D106" s="10" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="107" spans="1:4">
@@ -5300,11 +5434,11 @@
         <v>106</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C107" s="4"/>
       <c r="D107" s="14" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -5312,13 +5446,13 @@
         <v>107</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D108" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="109" spans="1:4">
@@ -5326,11 +5460,11 @@
         <v>108</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C109" s="4"/>
       <c r="D109" s="14" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -5338,11 +5472,11 @@
         <v>109</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C110" s="4"/>
       <c r="D110" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="111" spans="1:4">
@@ -5350,13 +5484,13 @@
         <v>110</v>
       </c>
       <c r="B111" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="C111" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="C111" s="4" t="s">
+      <c r="D111" s="14" t="s">
         <v>270</v>
-      </c>
-      <c r="D111" s="14" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -5364,11 +5498,11 @@
         <v>111</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C112" s="4"/>
       <c r="D112" s="14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="113" spans="1:4">
@@ -5376,11 +5510,11 @@
         <v>112</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C113" s="4"/>
       <c r="D113" s="14" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -5388,13 +5522,13 @@
         <v>113</v>
       </c>
       <c r="B114" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="C114" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="C114" s="4" t="s">
+      <c r="D114" s="14" t="s">
         <v>277</v>
-      </c>
-      <c r="D114" s="14" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -5402,11 +5536,11 @@
         <v>114</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C115" s="4"/>
       <c r="D115" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -5414,13 +5548,13 @@
         <v>115</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D116" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -5428,11 +5562,11 @@
         <v>116</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C117" s="4"/>
       <c r="D117" s="14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -5440,11 +5574,11 @@
         <v>117</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C118" s="4"/>
       <c r="D118" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -5452,13 +5586,13 @@
         <v>118</v>
       </c>
       <c r="B119" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="C119" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="C119" s="4" t="s">
+      <c r="D119" s="14" t="s">
         <v>289</v>
-      </c>
-      <c r="D119" s="14" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -5466,11 +5600,11 @@
         <v>119</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C120" s="4"/>
       <c r="D120" s="15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -5478,11 +5612,11 @@
         <v>120</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C121" s="4"/>
       <c r="D121" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -5490,13 +5624,13 @@
         <v>121</v>
       </c>
       <c r="B122" s="9" t="s">
+        <v>388</v>
+      </c>
+      <c r="C122" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="C122" s="4" t="s">
-        <v>390</v>
-      </c>
       <c r="D122" s="15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -5504,13 +5638,13 @@
         <v>122</v>
       </c>
       <c r="B123" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C123" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="D123" s="14" t="s">
         <v>296</v>
-      </c>
-      <c r="C123" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="D123" s="14" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -5518,11 +5652,11 @@
         <v>123</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C124" s="4"/>
       <c r="D124" s="14" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -5530,11 +5664,11 @@
         <v>124</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C125" s="4"/>
       <c r="D125" s="14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="126" spans="1:4">
@@ -5542,11 +5676,11 @@
         <v>125</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C126" s="4"/>
       <c r="D126" s="14" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -5554,13 +5688,13 @@
         <v>126</v>
       </c>
       <c r="B127" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="C127" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="C127" s="4" t="s">
+      <c r="D127" s="14" t="s">
         <v>306</v>
-      </c>
-      <c r="D127" s="14" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -5568,11 +5702,11 @@
         <v>127</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C128" s="4"/>
       <c r="D128" s="14" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="129" spans="1:4">
@@ -5580,11 +5714,11 @@
         <v>128</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C129" s="4"/>
       <c r="D129" s="14" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -5592,11 +5726,11 @@
         <v>129</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C130" s="4"/>
       <c r="D130" s="14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="131" spans="1:4">
@@ -5604,13 +5738,13 @@
         <v>130</v>
       </c>
       <c r="B131" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C131" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="D131" s="14" t="s">
         <v>314</v>
-      </c>
-      <c r="C131" s="4" t="s">
-        <v>316</v>
-      </c>
-      <c r="D131" s="14" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -5618,11 +5752,11 @@
         <v>131</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C132" s="4"/>
       <c r="D132" s="14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -5630,11 +5764,11 @@
         <v>132</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C133" s="4"/>
       <c r="D133" s="14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="134" spans="1:4">
@@ -5642,11 +5776,11 @@
         <v>133</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C134" s="4"/>
       <c r="D134" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="135" spans="1:4">
@@ -5654,11 +5788,11 @@
         <v>134</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C135" s="4"/>
       <c r="D135" s="14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="136" spans="1:4">
@@ -5666,13 +5800,13 @@
         <v>135</v>
       </c>
       <c r="B136" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="C136" s="4" t="s">
         <v>323</v>
       </c>
-      <c r="C136" s="4" t="s">
+      <c r="D136" s="14" t="s">
         <v>324</v>
-      </c>
-      <c r="D136" s="14" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -5680,11 +5814,11 @@
         <v>136</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C137" s="4"/>
       <c r="D137" s="14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="138" spans="1:4">
@@ -5692,11 +5826,11 @@
         <v>137</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C138" s="4"/>
       <c r="D138" s="15" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="139" spans="1:4">
@@ -5704,11 +5838,11 @@
         <v>138</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C139" s="4"/>
       <c r="D139" s="14" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="140" spans="1:4">
@@ -5716,13 +5850,13 @@
         <v>139</v>
       </c>
       <c r="B140" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="C140" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="D140" s="14" t="s">
         <v>332</v>
-      </c>
-      <c r="C140" s="4" t="s">
-        <v>339</v>
-      </c>
-      <c r="D140" s="14" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -5730,11 +5864,11 @@
         <v>140</v>
       </c>
       <c r="B141" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C141" s="4"/>
       <c r="D141" s="14" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="142" spans="1:4">
@@ -5742,13 +5876,13 @@
         <v>141</v>
       </c>
       <c r="B142" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="C142" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="D142" s="15" t="s">
         <v>336</v>
-      </c>
-      <c r="C142" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="D142" s="15" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -5756,13 +5890,13 @@
         <v>142</v>
       </c>
       <c r="B143" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="C143" s="4" t="s">
         <v>340</v>
       </c>
-      <c r="C143" s="4" t="s">
+      <c r="D143" s="14" t="s">
         <v>341</v>
-      </c>
-      <c r="D143" s="14" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -5770,11 +5904,11 @@
         <v>143</v>
       </c>
       <c r="B144" s="4" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C144" s="4"/>
       <c r="D144" s="14" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -5782,11 +5916,11 @@
         <v>144</v>
       </c>
       <c r="B145" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C145" s="4"/>
       <c r="D145" s="14" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -5794,11 +5928,11 @@
         <v>145</v>
       </c>
       <c r="B146" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C146" s="4"/>
       <c r="D146" s="14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="147" spans="1:5" ht="38">
@@ -5806,16 +5940,16 @@
         <v>146</v>
       </c>
       <c r="B147" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="C147" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="C147" s="4" t="s">
+      <c r="D147" s="14" t="s">
         <v>350</v>
       </c>
-      <c r="D147" s="14" t="s">
-        <v>351</v>
-      </c>
       <c r="E147" s="17" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -5823,11 +5957,11 @@
         <v>147</v>
       </c>
       <c r="B148" s="4" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C148" s="4"/>
       <c r="D148" s="14" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -5835,13 +5969,13 @@
         <v>148</v>
       </c>
       <c r="B149" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="C149" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="D149" s="14" t="s">
         <v>354</v>
-      </c>
-      <c r="C149" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="D149" s="14" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -5849,13 +5983,13 @@
         <v>149</v>
       </c>
       <c r="B150" s="4" t="s">
+        <v>356</v>
+      </c>
+      <c r="C150" s="4" t="s">
         <v>357</v>
       </c>
-      <c r="C150" s="4" t="s">
-        <v>358</v>
-      </c>
       <c r="D150" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -5863,13 +5997,13 @@
         <v>150</v>
       </c>
       <c r="B151" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="C151" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="C151" s="4" t="s">
+      <c r="D151" s="15" t="s">
         <v>361</v>
-      </c>
-      <c r="D151" s="15" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -5877,11 +6011,11 @@
         <v>151</v>
       </c>
       <c r="B152" s="9" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C152" s="4"/>
       <c r="D152" s="15" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -5889,11 +6023,11 @@
         <v>152</v>
       </c>
       <c r="B153" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C153" s="4"/>
       <c r="D153" s="15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -5901,11 +6035,11 @@
         <v>153</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C154" s="4"/>
       <c r="D154" s="14" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -5913,11 +6047,11 @@
         <v>154</v>
       </c>
       <c r="B155" s="4" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C155" s="4"/>
       <c r="D155" s="14" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -5925,11 +6059,11 @@
         <v>155</v>
       </c>
       <c r="B156" s="4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C156" s="4"/>
       <c r="D156" s="14" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="157" spans="1:5">
@@ -5937,13 +6071,13 @@
         <v>156</v>
       </c>
       <c r="B157" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="C157" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="D157" s="14" t="s">
         <v>373</v>
-      </c>
-      <c r="C157" s="4" t="s">
-        <v>375</v>
-      </c>
-      <c r="D157" s="14" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="158" spans="1:5">
@@ -5951,11 +6085,11 @@
         <v>157</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C158" s="4"/>
       <c r="D158" s="14" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="159" spans="1:5">
@@ -5963,13 +6097,13 @@
         <v>158</v>
       </c>
       <c r="B159" s="9" t="s">
+        <v>377</v>
+      </c>
+      <c r="C159" s="9" t="s">
         <v>378</v>
       </c>
-      <c r="C159" s="9" t="s">
+      <c r="D159" s="15" t="s">
         <v>379</v>
-      </c>
-      <c r="D159" s="15" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="160" spans="1:5">
@@ -5977,11 +6111,11 @@
         <v>159</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C160" s="4"/>
       <c r="D160" s="14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -5989,13 +6123,13 @@
         <v>160</v>
       </c>
       <c r="B161" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="C161" s="4" t="s">
         <v>384</v>
       </c>
-      <c r="C161" s="4" t="s">
-        <v>385</v>
-      </c>
       <c r="D161" s="14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -6003,13 +6137,13 @@
         <v>161</v>
       </c>
       <c r="B162" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="C162" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="D162" s="14" t="s">
         <v>386</v>
-      </c>
-      <c r="C162" s="4" t="s">
-        <v>388</v>
-      </c>
-      <c r="D162" s="14" t="s">
-        <v>387</v>
       </c>
     </row>
     <row r="163" spans="1:4">
@@ -6017,11 +6151,11 @@
         <v>162</v>
       </c>
       <c r="B163" s="4" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C163" s="4"/>
       <c r="D163" s="14" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -6029,11 +6163,11 @@
         <v>163</v>
       </c>
       <c r="B164" s="4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C164" s="4"/>
       <c r="D164" s="14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -6041,13 +6175,13 @@
         <v>164</v>
       </c>
       <c r="B165" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="C165" s="4" t="s">
         <v>395</v>
       </c>
-      <c r="C165" s="4" t="s">
+      <c r="D165" s="14" t="s">
         <v>396</v>
-      </c>
-      <c r="D165" s="14" t="s">
-        <v>397</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -6055,13 +6189,13 @@
         <v>165</v>
       </c>
       <c r="B166" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="C166" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="D166" s="14" t="s">
         <v>398</v>
-      </c>
-      <c r="C166" s="4" t="s">
-        <v>400</v>
-      </c>
-      <c r="D166" s="14" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="167" spans="1:4">
@@ -6069,11 +6203,11 @@
         <v>166</v>
       </c>
       <c r="B167" s="4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C167" s="4"/>
       <c r="D167" s="14" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -6081,13 +6215,13 @@
         <v>167</v>
       </c>
       <c r="B168" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="C168" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="D168" s="14" t="s">
         <v>403</v>
-      </c>
-      <c r="C168" s="4" t="s">
-        <v>405</v>
-      </c>
-      <c r="D168" s="14" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -6095,13 +6229,13 @@
         <v>168</v>
       </c>
       <c r="B169" s="9" t="s">
+        <v>405</v>
+      </c>
+      <c r="C169" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="D169" s="15" t="s">
         <v>406</v>
-      </c>
-      <c r="C169" s="4" t="s">
-        <v>408</v>
-      </c>
-      <c r="D169" s="15" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -6109,13 +6243,13 @@
         <v>169</v>
       </c>
       <c r="B170" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="C170" s="4" t="s">
         <v>409</v>
       </c>
-      <c r="C170" s="4" t="s">
+      <c r="D170" s="15" t="s">
         <v>410</v>
-      </c>
-      <c r="D170" s="15" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -6123,11 +6257,11 @@
         <v>170</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C171" s="4"/>
       <c r="D171" s="14" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -6135,11 +6269,11 @@
         <v>171</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C172" s="4"/>
       <c r="D172" s="14" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -6147,11 +6281,11 @@
         <v>172</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C173" s="4"/>
       <c r="D173" s="14" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="174" spans="1:4">
@@ -6159,13 +6293,13 @@
         <v>173</v>
       </c>
       <c r="B174" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C174" s="4" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D174" s="15" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -6173,13 +6307,13 @@
         <v>174</v>
       </c>
       <c r="B175" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="C175" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="D175" s="14" t="s">
         <v>420</v>
-      </c>
-      <c r="C175" s="4" t="s">
-        <v>422</v>
-      </c>
-      <c r="D175" s="14" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -6187,13 +6321,13 @@
         <v>175</v>
       </c>
       <c r="B176" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="C176" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D176" s="14" t="s">
         <v>423</v>
-      </c>
-      <c r="C176" s="4" t="s">
-        <v>425</v>
-      </c>
-      <c r="D176" s="14" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="177" spans="1:8">
@@ -6201,13 +6335,13 @@
         <v>176</v>
       </c>
       <c r="B177" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="C177" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="D177" s="14" t="s">
         <v>426</v>
-      </c>
-      <c r="C177" s="4" t="s">
-        <v>428</v>
-      </c>
-      <c r="D177" s="14" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="178" spans="1:8">
@@ -6215,11 +6349,11 @@
         <v>177</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C178" s="4"/>
       <c r="D178" s="14" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="179" spans="1:8">
@@ -6227,13 +6361,13 @@
         <v>178</v>
       </c>
       <c r="B179" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="C179" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="D179" s="14" t="s">
         <v>431</v>
-      </c>
-      <c r="C179" s="4" t="s">
-        <v>433</v>
-      </c>
-      <c r="D179" s="14" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="180" spans="1:8">
@@ -6241,13 +6375,13 @@
         <v>179</v>
       </c>
       <c r="B180" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="C180" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="D180" s="14" t="s">
         <v>434</v>
-      </c>
-      <c r="C180" s="4" t="s">
-        <v>439</v>
-      </c>
-      <c r="D180" s="14" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="181" spans="1:8">
@@ -6255,13 +6389,13 @@
         <v>180</v>
       </c>
       <c r="B181" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="C181" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="D181" s="14" t="s">
         <v>436</v>
-      </c>
-      <c r="C181" s="4" t="s">
-        <v>438</v>
-      </c>
-      <c r="D181" s="14" t="s">
-        <v>437</v>
       </c>
     </row>
     <row r="182" spans="1:8">
@@ -6269,13 +6403,13 @@
         <v>181</v>
       </c>
       <c r="B182" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="C182" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="D182" s="14" t="s">
         <v>440</v>
-      </c>
-      <c r="C182" s="4" t="s">
-        <v>442</v>
-      </c>
-      <c r="D182" s="14" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="183" spans="1:8">
@@ -6283,11 +6417,11 @@
         <v>182</v>
       </c>
       <c r="B183" s="4" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C183" s="4"/>
       <c r="D183" s="14" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="184" spans="1:8">
@@ -6295,13 +6429,13 @@
         <v>183</v>
       </c>
       <c r="B184" s="4" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C184" s="4" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D184" s="14" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="185" spans="1:8">
@@ -6309,11 +6443,11 @@
         <v>184</v>
       </c>
       <c r="B185" s="4" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C185" s="4"/>
       <c r="D185" s="14" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="186" spans="1:8">
@@ -6321,11 +6455,11 @@
         <v>185</v>
       </c>
       <c r="B186" s="4" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C186" s="4"/>
       <c r="D186" s="14" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="187" spans="1:8">
@@ -6333,13 +6467,13 @@
         <v>186</v>
       </c>
       <c r="B187" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="C187" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="D187" s="14" t="s">
         <v>452</v>
-      </c>
-      <c r="C187" s="4" t="s">
-        <v>456</v>
-      </c>
-      <c r="D187" s="14" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="188" spans="1:8">
@@ -6347,13 +6481,13 @@
         <v>187</v>
       </c>
       <c r="B188" s="9" t="s">
+        <v>453</v>
+      </c>
+      <c r="C188" s="9" t="s">
+        <v>456</v>
+      </c>
+      <c r="D188" s="15" t="s">
         <v>454</v>
-      </c>
-      <c r="C188" s="9" t="s">
-        <v>457</v>
-      </c>
-      <c r="D188" s="15" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="189" spans="1:8">
@@ -6361,13 +6495,13 @@
         <v>188</v>
       </c>
       <c r="B189" s="4" t="s">
+        <v>458</v>
+      </c>
+      <c r="C189" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="D189" s="14" t="s">
         <v>459</v>
-      </c>
-      <c r="C189" s="4" t="s">
-        <v>461</v>
-      </c>
-      <c r="D189" s="14" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="190" spans="1:8">
@@ -6375,11 +6509,11 @@
         <v>189</v>
       </c>
       <c r="B190" s="4" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C190" s="4"/>
       <c r="D190" s="14" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="191" spans="1:8">
@@ -6387,14 +6521,14 @@
         <v>190</v>
       </c>
       <c r="B191" s="4" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C191" s="4"/>
       <c r="D191" s="14" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="H191" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="192" spans="1:8">
@@ -6402,11 +6536,11 @@
         <v>191</v>
       </c>
       <c r="B192" s="4" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C192" s="4"/>
       <c r="D192" s="14" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="193" spans="1:4">
@@ -6414,10 +6548,10 @@
         <v>192</v>
       </c>
       <c r="B193" s="4" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D193" s="14" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="194" spans="1:4">
@@ -6425,11 +6559,11 @@
         <v>193</v>
       </c>
       <c r="B194" s="4" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C194" s="4"/>
       <c r="D194" s="14" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="195" spans="1:4">
@@ -6437,11 +6571,11 @@
         <v>194</v>
       </c>
       <c r="B195" s="4" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C195" s="4"/>
       <c r="D195" s="14" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="196" spans="1:4">
@@ -6449,11 +6583,11 @@
         <v>195</v>
       </c>
       <c r="B196" s="4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C196" s="4"/>
       <c r="D196" s="14" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="197" spans="1:4">
@@ -6461,13 +6595,13 @@
         <v>196</v>
       </c>
       <c r="B197" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="C197" s="4" t="s">
         <v>477</v>
       </c>
-      <c r="C197" s="4" t="s">
-        <v>478</v>
-      </c>
       <c r="D197" s="14" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="198" spans="1:4">
@@ -6475,11 +6609,11 @@
         <v>197</v>
       </c>
       <c r="B198" s="4" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C198" s="4"/>
       <c r="D198" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="199" spans="1:4">
@@ -6487,11 +6621,11 @@
         <v>198</v>
       </c>
       <c r="B199" s="9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C199" s="4"/>
       <c r="D199" s="14" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="200" spans="1:4">
@@ -6499,11 +6633,11 @@
         <v>199</v>
       </c>
       <c r="B200" s="4" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C200" s="4"/>
       <c r="D200" s="14" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="201" spans="1:4">
@@ -6511,11 +6645,11 @@
         <v>200</v>
       </c>
       <c r="B201" s="9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C201" s="4"/>
       <c r="D201" s="14" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="202" spans="1:4">
@@ -6523,11 +6657,11 @@
         <v>201</v>
       </c>
       <c r="B202" s="4" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C202" s="4"/>
       <c r="D202" s="14" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -6535,11 +6669,11 @@
         <v>202</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C203" s="4"/>
       <c r="D203" s="14" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="204" spans="1:4">
@@ -6547,11 +6681,11 @@
         <v>203</v>
       </c>
       <c r="B204" s="4" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C204" s="4"/>
       <c r="D204" s="14" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="205" spans="1:4">
@@ -6559,11 +6693,11 @@
         <v>204</v>
       </c>
       <c r="B205" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C205" s="4"/>
       <c r="D205" s="14" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -6571,13 +6705,13 @@
         <v>205</v>
       </c>
       <c r="B206" s="9" t="s">
+        <v>492</v>
+      </c>
+      <c r="C206" s="4" t="s">
         <v>493</v>
       </c>
-      <c r="C206" s="4" t="s">
-        <v>494</v>
-      </c>
       <c r="D206" s="14" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="207" spans="1:4">
@@ -6585,11 +6719,11 @@
         <v>206</v>
       </c>
       <c r="B207" s="4" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C207" s="4"/>
       <c r="D207" s="14" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="208" spans="1:4">
@@ -6597,11 +6731,11 @@
         <v>207</v>
       </c>
       <c r="B208" s="4" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C208" s="4"/>
       <c r="D208" s="14" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="209" spans="1:4">
@@ -6609,11 +6743,11 @@
         <v>208</v>
       </c>
       <c r="B209" s="4" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C209" s="4"/>
       <c r="D209" s="14" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="210" spans="1:4">
@@ -6621,13 +6755,13 @@
         <v>209</v>
       </c>
       <c r="B210" s="4" t="s">
+        <v>501</v>
+      </c>
+      <c r="C210" s="4" t="s">
+        <v>503</v>
+      </c>
+      <c r="D210" s="14" t="s">
         <v>502</v>
-      </c>
-      <c r="C210" s="4" t="s">
-        <v>504</v>
-      </c>
-      <c r="D210" s="14" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="211" spans="1:4">
@@ -6635,11 +6769,11 @@
         <v>210</v>
       </c>
       <c r="B211" s="4" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C211" s="4"/>
       <c r="D211" s="14" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="212" spans="1:4">
@@ -6647,11 +6781,11 @@
         <v>211</v>
       </c>
       <c r="B212" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="C212" s="4"/>
       <c r="D212" s="14" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="213" spans="1:4">
@@ -6659,13 +6793,13 @@
         <v>212</v>
       </c>
       <c r="B213" s="4" t="s">
+        <v>508</v>
+      </c>
+      <c r="C213" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="D213" s="14" t="s">
         <v>509</v>
-      </c>
-      <c r="C213" s="4" t="s">
-        <v>511</v>
-      </c>
-      <c r="D213" s="14" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="214" spans="1:4">
@@ -6673,11 +6807,11 @@
         <v>213</v>
       </c>
       <c r="B214" s="9" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C214" s="4"/>
       <c r="D214" s="15" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="215" spans="1:4">
@@ -6685,11 +6819,11 @@
         <v>214</v>
       </c>
       <c r="B215" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C215" s="4"/>
       <c r="D215" s="14" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="216" spans="1:4">
@@ -6697,13 +6831,13 @@
         <v>215</v>
       </c>
       <c r="B216" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="C216" s="4" t="s">
+        <v>517</v>
+      </c>
+      <c r="D216" s="14" t="s">
         <v>516</v>
-      </c>
-      <c r="C216" s="4" t="s">
-        <v>518</v>
-      </c>
-      <c r="D216" s="14" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="217" spans="1:4">
@@ -6711,13 +6845,13 @@
         <v>216</v>
       </c>
       <c r="B217" s="4" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C217" s="4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D217" s="14" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="218" spans="1:4">
@@ -6725,13 +6859,13 @@
         <v>217</v>
       </c>
       <c r="B218" s="4" t="s">
+        <v>519</v>
+      </c>
+      <c r="C218" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="D218" s="14" t="s">
         <v>520</v>
-      </c>
-      <c r="C218" s="4" t="s">
-        <v>522</v>
-      </c>
-      <c r="D218" s="14" t="s">
-        <v>521</v>
       </c>
     </row>
     <row r="219" spans="1:4">
@@ -6739,11 +6873,11 @@
         <v>218</v>
       </c>
       <c r="B219" s="9" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C219" s="4"/>
       <c r="D219" s="15" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="220" spans="1:4">
@@ -6751,11 +6885,11 @@
         <v>219</v>
       </c>
       <c r="B220" s="4" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C220" s="4"/>
       <c r="D220" s="14" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="221" spans="1:4">
@@ -6763,11 +6897,11 @@
         <v>220</v>
       </c>
       <c r="B221" s="4" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C221" s="4"/>
       <c r="D221" s="14" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="222" spans="1:4">
@@ -6775,11 +6909,11 @@
         <v>221</v>
       </c>
       <c r="B222" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C222" s="4"/>
       <c r="D222" s="14" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="223" spans="1:4">
@@ -6787,11 +6921,11 @@
         <v>222</v>
       </c>
       <c r="B223" s="4" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C223" s="4"/>
       <c r="D223" s="14" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="224" spans="1:4">
@@ -6799,11 +6933,11 @@
         <v>223</v>
       </c>
       <c r="B224" s="4" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C224" s="4"/>
       <c r="D224" s="14" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="225" spans="1:5">
@@ -6811,11 +6945,11 @@
         <v>224</v>
       </c>
       <c r="B225" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C225" s="4"/>
       <c r="D225" s="14" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="226" spans="1:5">
@@ -6823,11 +6957,11 @@
         <v>225</v>
       </c>
       <c r="B226" s="4" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C226" s="4"/>
       <c r="D226" s="14" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="227" spans="1:5">
@@ -6835,11 +6969,11 @@
         <v>226</v>
       </c>
       <c r="B227" s="4" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C227" s="4"/>
       <c r="D227" s="14" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="228" spans="1:5">
@@ -6847,11 +6981,11 @@
         <v>227</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C228" s="4"/>
       <c r="D228" s="14" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="229" spans="1:5">
@@ -6859,11 +6993,11 @@
         <v>228</v>
       </c>
       <c r="B229" s="4" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C229" s="4"/>
       <c r="D229" s="14" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="230" spans="1:5">
@@ -6871,11 +7005,11 @@
         <v>229</v>
       </c>
       <c r="B230" s="4" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C230" s="4"/>
       <c r="D230" s="14" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="231" spans="1:5">
@@ -6883,11 +7017,11 @@
         <v>230</v>
       </c>
       <c r="B231" s="4" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C231" s="4"/>
       <c r="D231" s="14" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="232" spans="1:5">
@@ -6895,11 +7029,11 @@
         <v>231</v>
       </c>
       <c r="B232" s="4" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C232" s="4"/>
       <c r="D232" s="14" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="233" spans="1:5" ht="72" customHeight="1">
@@ -6907,14 +7041,14 @@
         <v>232</v>
       </c>
       <c r="B233" s="4" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C233" s="4"/>
       <c r="D233" s="14" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E233" s="17" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="234" spans="1:5" ht="38">
@@ -6922,14 +7056,14 @@
         <v>233</v>
       </c>
       <c r="B234" s="4" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C234" s="4"/>
       <c r="D234" s="14" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="E234" s="17" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="235" spans="1:5" ht="57">
@@ -6937,14 +7071,14 @@
         <v>234</v>
       </c>
       <c r="B235" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="C235" s="4"/>
       <c r="D235" s="14" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="E235" s="17" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="236" spans="1:5" ht="57">
@@ -6952,14 +7086,14 @@
         <v>235</v>
       </c>
       <c r="B236" s="4" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C236" s="4"/>
       <c r="D236" s="14" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="E236" s="17" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="237" spans="1:5" ht="57">
@@ -6967,16 +7101,16 @@
         <v>236</v>
       </c>
       <c r="B237" s="9" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C237" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D237" s="14" t="s">
+        <v>564</v>
+      </c>
+      <c r="E237" s="17" t="s">
         <v>565</v>
-      </c>
-      <c r="E237" s="17" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="238" spans="1:5" ht="57">
@@ -6984,14 +7118,14 @@
         <v>237</v>
       </c>
       <c r="B238" s="9" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C238" s="4"/>
       <c r="D238" s="14" t="s">
+        <v>568</v>
+      </c>
+      <c r="E238" s="17" t="s">
         <v>569</v>
-      </c>
-      <c r="E238" s="17" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="239" spans="1:5" ht="71" customHeight="1">
@@ -6999,14 +7133,14 @@
         <v>238</v>
       </c>
       <c r="B239" s="4" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="C239" s="4"/>
       <c r="D239" s="14" t="s">
+        <v>571</v>
+      </c>
+      <c r="E239" s="17" t="s">
         <v>572</v>
-      </c>
-      <c r="E239" s="17" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="240" spans="1:5" ht="95">
@@ -7014,14 +7148,14 @@
         <v>239</v>
       </c>
       <c r="B240" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="C240" s="4"/>
       <c r="D240" s="14" t="s">
+        <v>574</v>
+      </c>
+      <c r="E240" s="17" t="s">
         <v>575</v>
-      </c>
-      <c r="E240" s="17" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="241" spans="1:5" ht="57">
@@ -7029,14 +7163,14 @@
         <v>240</v>
       </c>
       <c r="B241" s="4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C241" s="4"/>
       <c r="D241" s="14" t="s">
+        <v>577</v>
+      </c>
+      <c r="E241" s="17" t="s">
         <v>578</v>
-      </c>
-      <c r="E241" s="17" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="242" spans="1:5" ht="57">
@@ -7044,14 +7178,14 @@
         <v>241</v>
       </c>
       <c r="B242" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C242" s="4"/>
       <c r="D242" s="14" t="s">
+        <v>580</v>
+      </c>
+      <c r="E242" s="17" t="s">
         <v>581</v>
-      </c>
-      <c r="E242" s="17" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="243" spans="1:5" ht="38">
@@ -7061,10 +7195,10 @@
       <c r="B243" s="4"/>
       <c r="C243" s="4"/>
       <c r="D243" s="14" t="s">
+        <v>582</v>
+      </c>
+      <c r="E243" s="17" t="s">
         <v>583</v>
-      </c>
-      <c r="E243" s="17" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="244" spans="1:5" ht="76">
@@ -7072,14 +7206,14 @@
         <v>243</v>
       </c>
       <c r="B244" s="4" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="C244" s="4"/>
       <c r="D244" s="14" t="s">
+        <v>585</v>
+      </c>
+      <c r="E244" s="17" t="s">
         <v>586</v>
-      </c>
-      <c r="E244" s="17" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="245" spans="1:5" ht="57">
@@ -7087,14 +7221,14 @@
         <v>244</v>
       </c>
       <c r="B245" s="4" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="C245" s="4"/>
       <c r="D245" s="12" t="s">
+        <v>588</v>
+      </c>
+      <c r="E245" s="17" t="s">
         <v>589</v>
-      </c>
-      <c r="E245" s="17" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="246" spans="1:5" ht="38">
@@ -7102,14 +7236,14 @@
         <v>245</v>
       </c>
       <c r="B246" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C246" s="4"/>
       <c r="D246" s="12" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E246" s="17" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="247" spans="1:5" ht="38">
@@ -7117,14 +7251,14 @@
         <v>246</v>
       </c>
       <c r="B247" s="4" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C247" s="4"/>
       <c r="D247" s="12" t="s">
+        <v>593</v>
+      </c>
+      <c r="E247" s="17" t="s">
         <v>594</v>
-      </c>
-      <c r="E247" s="17" t="s">
-        <v>595</v>
       </c>
     </row>
     <row r="248" spans="1:5" ht="76">
@@ -7132,14 +7266,14 @@
         <v>247</v>
       </c>
       <c r="B248" s="4" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="C248" s="4"/>
       <c r="D248" s="12" t="s">
+        <v>596</v>
+      </c>
+      <c r="E248" s="17" t="s">
         <v>597</v>
-      </c>
-      <c r="E248" s="17" t="s">
-        <v>598</v>
       </c>
     </row>
     <row r="249" spans="1:5" ht="38">
@@ -7147,16 +7281,16 @@
         <v>248</v>
       </c>
       <c r="B249" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="C249" s="4" t="s">
         <v>599</v>
       </c>
-      <c r="C249" s="4" t="s">
+      <c r="D249" s="12" t="s">
         <v>600</v>
       </c>
-      <c r="D249" s="12" t="s">
+      <c r="E249" s="17" t="s">
         <v>601</v>
-      </c>
-      <c r="E249" s="17" t="s">
-        <v>602</v>
       </c>
     </row>
     <row r="250" spans="1:5" ht="111" customHeight="1">
@@ -7164,16 +7298,16 @@
         <v>249</v>
       </c>
       <c r="B250" s="3" t="s">
+        <v>602</v>
+      </c>
+      <c r="C250" s="3" t="s">
+        <v>605</v>
+      </c>
+      <c r="D250" s="12" t="s">
         <v>603</v>
       </c>
-      <c r="C250" s="3" t="s">
-        <v>606</v>
-      </c>
-      <c r="D250" s="12" t="s">
+      <c r="E250" s="17" t="s">
         <v>604</v>
-      </c>
-      <c r="E250" s="17" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="251" spans="1:5" ht="38">
@@ -7181,14 +7315,14 @@
         <v>250</v>
       </c>
       <c r="B251" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C251" s="3"/>
       <c r="D251" s="12" t="s">
+        <v>607</v>
+      </c>
+      <c r="E251" s="17" t="s">
         <v>608</v>
-      </c>
-      <c r="E251" s="17" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="252" spans="1:5" ht="71" customHeight="1">
@@ -7196,14 +7330,14 @@
         <v>251</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="C252" s="3"/>
       <c r="D252" s="12" t="s">
+        <v>610</v>
+      </c>
+      <c r="E252" s="17" t="s">
         <v>611</v>
-      </c>
-      <c r="E252" s="17" t="s">
-        <v>612</v>
       </c>
     </row>
     <row r="253" spans="1:5" ht="76">
@@ -7211,14 +7345,14 @@
         <v>252</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="C253" s="3"/>
       <c r="D253" s="12" t="s">
+        <v>613</v>
+      </c>
+      <c r="E253" s="17" t="s">
         <v>614</v>
-      </c>
-      <c r="E253" s="17" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="254" spans="1:5" ht="57">
@@ -7226,14 +7360,14 @@
         <v>253</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="C254" s="3"/>
       <c r="D254" s="12" t="s">
+        <v>616</v>
+      </c>
+      <c r="E254" s="17" t="s">
         <v>617</v>
-      </c>
-      <c r="E254" s="17" t="s">
-        <v>618</v>
       </c>
     </row>
     <row r="255" spans="1:5" ht="76">
@@ -7241,14 +7375,14 @@
         <v>254</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="C255" s="3"/>
       <c r="D255" s="12" t="s">
+        <v>619</v>
+      </c>
+      <c r="E255" s="17" t="s">
         <v>620</v>
-      </c>
-      <c r="E255" s="17" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="256" spans="1:5" ht="95">
@@ -7256,16 +7390,16 @@
         <v>255</v>
       </c>
       <c r="B256" s="3" t="s">
+        <v>621</v>
+      </c>
+      <c r="C256" s="3" t="s">
+        <v>623</v>
+      </c>
+      <c r="D256" s="12" t="s">
         <v>622</v>
       </c>
-      <c r="C256" s="3" t="s">
+      <c r="E256" s="17" t="s">
         <v>624</v>
-      </c>
-      <c r="D256" s="12" t="s">
-        <v>623</v>
-      </c>
-      <c r="E256" s="17" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="257" spans="1:5" ht="109" customHeight="1">
@@ -7273,14 +7407,14 @@
         <v>256</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C257" s="3"/>
       <c r="D257" s="12" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="E257" s="17" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="258" spans="1:5" ht="95">
@@ -7288,16 +7422,16 @@
         <v>257</v>
       </c>
       <c r="B258" s="3" t="s">
+        <v>629</v>
+      </c>
+      <c r="C258" s="3" t="s">
         <v>630</v>
       </c>
-      <c r="C258" s="3" t="s">
+      <c r="D258" s="12" t="s">
         <v>631</v>
       </c>
-      <c r="D258" s="12" t="s">
+      <c r="E258" s="17" t="s">
         <v>632</v>
-      </c>
-      <c r="E258" s="17" t="s">
-        <v>633</v>
       </c>
     </row>
     <row r="259" spans="1:5" ht="57">
@@ -7305,16 +7439,16 @@
         <v>258</v>
       </c>
       <c r="B259" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="C259" s="3" t="s">
+        <v>633</v>
+      </c>
+      <c r="D259" s="12" t="s">
         <v>634</v>
       </c>
-      <c r="D259" s="12" t="s">
+      <c r="E259" s="17" t="s">
         <v>635</v>
-      </c>
-      <c r="E259" s="17" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="260" spans="1:5" ht="57">
@@ -7322,14 +7456,14 @@
         <v>259</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="C260" s="3"/>
       <c r="D260" s="12" t="s">
+        <v>637</v>
+      </c>
+      <c r="E260" s="17" t="s">
         <v>638</v>
-      </c>
-      <c r="E260" s="17" t="s">
-        <v>639</v>
       </c>
     </row>
     <row r="261" spans="1:5" ht="57">
@@ -7337,16 +7471,16 @@
         <v>260</v>
       </c>
       <c r="B261" s="3" t="s">
+        <v>639</v>
+      </c>
+      <c r="C261" s="3" t="s">
+        <v>642</v>
+      </c>
+      <c r="D261" s="12" t="s">
         <v>640</v>
       </c>
-      <c r="C261" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="D261" s="12" t="s">
+      <c r="E261" s="17" t="s">
         <v>641</v>
-      </c>
-      <c r="E261" s="17" t="s">
-        <v>642</v>
       </c>
     </row>
     <row r="262" spans="1:5" ht="57">
@@ -7354,16 +7488,16 @@
         <v>261</v>
       </c>
       <c r="B262" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="C262" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="D262" s="12" t="s">
         <v>644</v>
       </c>
-      <c r="C262" s="3" t="s">
-        <v>647</v>
-      </c>
-      <c r="D262" s="12" t="s">
+      <c r="E262" s="17" t="s">
         <v>645</v>
-      </c>
-      <c r="E262" s="17" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="263" spans="1:5" ht="19">
@@ -7371,16 +7505,16 @@
         <v>262</v>
       </c>
       <c r="B263" s="3" t="s">
+        <v>647</v>
+      </c>
+      <c r="C263" s="3" t="s">
+        <v>652</v>
+      </c>
+      <c r="D263" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="E263" s="17" t="s">
         <v>648</v>
-      </c>
-      <c r="C263" s="3" t="s">
-        <v>653</v>
-      </c>
-      <c r="D263" s="12" t="s">
-        <v>241</v>
-      </c>
-      <c r="E263" s="17" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="264" spans="1:5" ht="19">
@@ -7388,16 +7522,16 @@
         <v>263</v>
       </c>
       <c r="B264" s="3" t="s">
+        <v>649</v>
+      </c>
+      <c r="C264" s="3" t="s">
+        <v>653</v>
+      </c>
+      <c r="D264" s="12" t="s">
         <v>650</v>
       </c>
-      <c r="C264" s="3" t="s">
-        <v>654</v>
-      </c>
-      <c r="D264" s="12" t="s">
+      <c r="E264" s="17" t="s">
         <v>651</v>
-      </c>
-      <c r="E264" s="17" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="265" spans="1:5" ht="57">
@@ -7405,16 +7539,16 @@
         <v>264</v>
       </c>
       <c r="B265" s="3" t="s">
+        <v>654</v>
+      </c>
+      <c r="C265" s="3" t="s">
+        <v>660</v>
+      </c>
+      <c r="D265" s="12" t="s">
+        <v>661</v>
+      </c>
+      <c r="E265" s="17" t="s">
         <v>655</v>
-      </c>
-      <c r="C265" s="3" t="s">
-        <v>661</v>
-      </c>
-      <c r="D265" s="12" t="s">
-        <v>662</v>
-      </c>
-      <c r="E265" s="17" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="266" spans="1:5" ht="114">
@@ -7422,41 +7556,66 @@
         <v>265</v>
       </c>
       <c r="B266" s="3" t="s">
+        <v>656</v>
+      </c>
+      <c r="C266" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="D266" s="12" t="s">
         <v>657</v>
       </c>
-      <c r="C266" s="3" t="s">
-        <v>660</v>
-      </c>
-      <c r="D266" s="12" t="s">
+      <c r="E266" s="17" t="s">
         <v>658</v>
       </c>
-      <c r="E266" s="17" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="267" spans="1:5">
+    </row>
+    <row r="267" spans="1:5" ht="95">
       <c r="A267" s="18">
         <v>266</v>
       </c>
-      <c r="B267" s="3"/>
-      <c r="C267" s="3"/>
-      <c r="D267" s="12"/>
-    </row>
-    <row r="268" spans="1:5">
+      <c r="B267" s="3" t="s">
+        <v>663</v>
+      </c>
+      <c r="C267" s="3" t="s">
+        <v>666</v>
+      </c>
+      <c r="D267" s="12" t="s">
+        <v>664</v>
+      </c>
+      <c r="E267" s="17" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" ht="94" customHeight="1">
       <c r="A268" s="18">
         <v>267</v>
       </c>
-      <c r="B268" s="3"/>
-      <c r="C268" s="3"/>
-      <c r="D268" s="12"/>
-    </row>
-    <row r="269" spans="1:5">
+      <c r="B268" s="3" t="s">
+        <v>667</v>
+      </c>
+      <c r="C268" s="3" t="s">
+        <v>668</v>
+      </c>
+      <c r="D268" s="12" t="s">
+        <v>669</v>
+      </c>
+      <c r="E268" s="17" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" ht="57">
       <c r="A269" s="18">
         <v>268</v>
       </c>
-      <c r="B269" s="3"/>
+      <c r="B269" s="3" t="s">
+        <v>672</v>
+      </c>
       <c r="C269" s="3"/>
-      <c r="D269" s="12"/>
+      <c r="D269" s="12" t="s">
+        <v>673</v>
+      </c>
+      <c r="E269" s="17" t="s">
+        <v>671</v>
+      </c>
     </row>
     <row r="270" spans="1:5">
       <c r="A270" s="18">

</xml_diff>

<commit_message>
update several MRE papers
</commit_message>
<xml_diff>
--- a/source/_posts/collection/new-words.xlsx
+++ b/source/_posts/collection/new-words.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuxiyang/myData/python-project/liuxiyang641.github.io/source/_posts/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5735D8BC-149F-DD4C-8E6B-7207337B10BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2175930-C229-1A4E-A96D-3DC9351E56D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33600" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{C07A63B5-5344-AF4A-AFD6-2139CC657E22}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="731" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="721">
   <si>
     <t>[rɪˈtriːvl]</t>
   </si>
@@ -4031,6 +4031,42 @@
   </si>
   <si>
     <t>发挥；施加</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>relieve</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>减轻；缓解</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> /rɪ'liːv/</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Distant supervision is an alternative method to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>relieve</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> this problem which leverages the alignment of knowledge bases and texts in sentences to automatically annotate relations.</t>
+    </r>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -4520,7 +4556,7 @@
   <dimension ref="A1:H696"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A280" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H290" sqref="H290"/>
+      <selection activeCell="G284" sqref="G284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -8293,13 +8329,22 @@
         <v>712</v>
       </c>
     </row>
-    <row r="282" spans="1:5">
+    <row r="282" spans="1:5" ht="95">
       <c r="A282" s="18">
         <v>281</v>
       </c>
-      <c r="B282" s="3"/>
-      <c r="C282" s="3"/>
-      <c r="D282" s="12"/>
+      <c r="B282" s="3" t="s">
+        <v>717</v>
+      </c>
+      <c r="C282" s="3" t="s">
+        <v>719</v>
+      </c>
+      <c r="D282" s="12" t="s">
+        <v>718</v>
+      </c>
+      <c r="E282" s="17" t="s">
+        <v>720</v>
+      </c>
     </row>
     <row r="283" spans="1:5">
       <c r="A283" s="18">

</xml_diff>

<commit_message>
add some new colloection of IE, data-augment papers
</commit_message>
<xml_diff>
--- a/source/_posts/collection/new-words.xlsx
+++ b/source/_posts/collection/new-words.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuxiyang/myData/python-project/liuxiyang641.github.io/source/_posts/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E094655C-0CFA-8D4C-A922-60EFA3435C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C494C47C-AC1A-B94F-BF08-DFEE2D43F310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33600" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{C07A63B5-5344-AF4A-AFD6-2139CC657E22}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="735">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="768">
   <si>
     <t>[rɪˈtriːvl]</t>
   </si>
@@ -4199,6 +4199,322 @@
         <family val="1"/>
       </rPr>
       <t xml:space="preserve"> to the above mentioned impediments</t>
+    </r>
+  </si>
+  <si>
+    <t>a borad range of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">可以用来替换a wide range of </t>
+  </si>
+  <si>
+    <r>
+      <t>In contrast to earlier PLMs, LLMs which consist of a significantly larger number of parameters require a higher volume of training data that covers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> a broad range of</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> content.</t>
+    </r>
+  </si>
+  <si>
+    <t>have a tendency to</t>
+  </si>
+  <si>
+    <t>可以用来替换tend to</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Moreover, LLMs </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>had a tendency to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> produce socially disruptive content...</t>
+    </r>
+  </si>
+  <si>
+    <t>non-exhaustive</t>
+  </si>
+  <si>
+    <t>非详尽无疑的</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Needless to say, applications covered in Figure 4 are </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>non-exhaustive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> considering the relentless speed and innovative zeal with which practitioners perpetually formulate both commercial and non-commercial ideas leveraging LLMs.</t>
+    </r>
+  </si>
+  <si>
+    <t>malicious</t>
+  </si>
+  <si>
+    <t>恶意的，心怀恶意的</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We define misinformation here as wrong information not intentionally generated by </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>malicious users</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to cause harm, but unintentionally generated by LLMs because they lack the ability to provide factually correct information.</t>
+    </r>
+  </si>
+  <si>
+    <t>exemplified</t>
+  </si>
+  <si>
+    <t>是…的典范，举例说明</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">This overconfidence, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>exemplified</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> in Figure 9, indicates the models’ lack of awareness regarding their outdated knowledge base about the question.</t>
+    </r>
+  </si>
+  <si>
+    <t>Hereinafter</t>
+  </si>
+  <si>
+    <t>（用于正文中的）在下文中</t>
+  </si>
+  <si>
+    <r>
+      <t>GPT-3 and its successor ChatGPT (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Hereinafter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> referred to collectively as GPT)</t>
+    </r>
+  </si>
+  <si>
+    <t>internalizing</t>
+  </si>
+  <si>
+    <t>内在化</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pre-trained large language models (LLMs), such as ChatGPT and LLaMA (Touvron et al., 2023a), have demonstrated impressive capabilities in </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>internalizing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> knowledge and responding to common inquiries.</t>
+    </r>
+  </si>
+  <si>
+    <t>In light of findings</t>
+  </si>
+  <si>
+    <t>鉴于这些发现</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>In light of these findings</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>, we envision the future of knowledge graphs and outline a research landscape.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We also observe that this phenomenon is more </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>pronounced</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> when we measure by traffic than by density.</t>
+    </r>
+  </si>
+  <si>
+    <t>pronounced</t>
+  </si>
+  <si>
+    <t>(现象)更加显著</t>
+  </si>
+  <si>
+    <t>inevitably</t>
+  </si>
+  <si>
+    <t>不可避免地，必然地</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">However, restructuring the syntactic structure of the original sentence </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>inevitably</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> breaks the coherence.</t>
+    </r>
+  </si>
+  <si>
+    <t>impede</t>
+  </si>
+  <si>
+    <t>阻碍，妨碍</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Augmentations that do not follow these patterns </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>impede</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> a NER model from learning such patterns effectively</t>
     </r>
   </si>
 </sst>
@@ -4687,8 +5003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B4733E-376B-124B-AFDB-49936A421CEF}">
   <dimension ref="A1:H696"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A283" zoomScale="125" workbookViewId="0">
-      <selection activeCell="G288" sqref="G288"/>
+    <sheetView tabSelected="1" topLeftCell="A294" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I312" sqref="I312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -8553,95 +8869,172 @@
         <v>734</v>
       </c>
     </row>
-    <row r="288" spans="1:5">
+    <row r="288" spans="1:5" ht="95">
       <c r="A288" s="18">
         <v>287</v>
       </c>
-      <c r="B288" s="3"/>
+      <c r="B288" s="3" t="s">
+        <v>735</v>
+      </c>
       <c r="C288" s="3"/>
-      <c r="D288" s="12"/>
-    </row>
-    <row r="289" spans="1:4">
+      <c r="D288" s="12" t="s">
+        <v>736</v>
+      </c>
+      <c r="E288" s="17" t="s">
+        <v>737</v>
+      </c>
+    </row>
+    <row r="289" spans="1:5" ht="38">
       <c r="A289" s="18">
         <v>288</v>
       </c>
-      <c r="B289" s="3"/>
+      <c r="B289" s="3" t="s">
+        <v>738</v>
+      </c>
       <c r="C289" s="3"/>
-      <c r="D289" s="12"/>
-    </row>
-    <row r="290" spans="1:4">
+      <c r="D289" s="12" t="s">
+        <v>739</v>
+      </c>
+      <c r="E289" s="17" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="290" spans="1:5" ht="114">
       <c r="A290" s="18">
         <v>289</v>
       </c>
-      <c r="B290" s="3"/>
+      <c r="B290" s="3" t="s">
+        <v>741</v>
+      </c>
       <c r="C290" s="3"/>
-      <c r="D290" s="12"/>
-    </row>
-    <row r="291" spans="1:4">
+      <c r="D290" s="12" t="s">
+        <v>742</v>
+      </c>
+      <c r="E290" s="17" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="291" spans="1:5" ht="114">
       <c r="A291" s="18">
         <v>290</v>
       </c>
-      <c r="B291" s="3"/>
+      <c r="B291" s="3" t="s">
+        <v>744</v>
+      </c>
       <c r="C291" s="3"/>
-      <c r="D291" s="12"/>
-    </row>
-    <row r="292" spans="1:4">
+      <c r="D291" s="12" t="s">
+        <v>745</v>
+      </c>
+      <c r="E291" s="17" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="292" spans="1:5" ht="76">
       <c r="A292" s="18">
         <v>291</v>
       </c>
-      <c r="B292" s="3"/>
+      <c r="B292" s="3" t="s">
+        <v>747</v>
+      </c>
       <c r="C292" s="3"/>
-      <c r="D292" s="12"/>
-    </row>
-    <row r="293" spans="1:4">
+      <c r="D292" s="12" t="s">
+        <v>748</v>
+      </c>
+      <c r="E292" s="17" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="293" spans="1:5" ht="57">
       <c r="A293" s="18">
         <v>292</v>
       </c>
-      <c r="B293" s="3"/>
+      <c r="B293" s="3" t="s">
+        <v>750</v>
+      </c>
       <c r="C293" s="3"/>
-      <c r="D293" s="12"/>
-    </row>
-    <row r="294" spans="1:4">
+      <c r="D293" s="12" t="s">
+        <v>751</v>
+      </c>
+      <c r="E293" s="17" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="294" spans="1:5" ht="114">
       <c r="A294" s="18">
         <v>293</v>
       </c>
-      <c r="B294" s="3"/>
+      <c r="B294" s="3" t="s">
+        <v>753</v>
+      </c>
       <c r="C294" s="3"/>
-      <c r="D294" s="12"/>
-    </row>
-    <row r="295" spans="1:4">
+      <c r="D294" s="12" t="s">
+        <v>754</v>
+      </c>
+      <c r="E294" s="17" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="295" spans="1:5" ht="57">
       <c r="A295" s="18">
         <v>294</v>
       </c>
-      <c r="B295" s="3"/>
+      <c r="B295" s="3" t="s">
+        <v>756</v>
+      </c>
       <c r="C295" s="3"/>
-      <c r="D295" s="12"/>
-    </row>
-    <row r="296" spans="1:4">
+      <c r="D295" s="12" t="s">
+        <v>757</v>
+      </c>
+      <c r="E295" s="17" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="296" spans="1:5" ht="57">
       <c r="A296" s="18">
         <v>295</v>
       </c>
-      <c r="B296" s="3"/>
+      <c r="B296" s="3" t="s">
+        <v>760</v>
+      </c>
       <c r="C296" s="3"/>
-      <c r="D296" s="12"/>
-    </row>
-    <row r="297" spans="1:4">
+      <c r="D296" s="12" t="s">
+        <v>761</v>
+      </c>
+      <c r="E296" s="17" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="297" spans="1:5" ht="57">
       <c r="A297" s="18">
         <v>296</v>
       </c>
-      <c r="B297" s="3"/>
+      <c r="B297" s="3" t="s">
+        <v>762</v>
+      </c>
       <c r="C297" s="3"/>
-      <c r="D297" s="12"/>
-    </row>
-    <row r="298" spans="1:4">
+      <c r="D297" s="12" t="s">
+        <v>763</v>
+      </c>
+      <c r="E297" s="17" t="s">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="298" spans="1:5" ht="57">
       <c r="A298" s="18">
         <v>297</v>
       </c>
-      <c r="B298" s="3"/>
+      <c r="B298" s="3" t="s">
+        <v>765</v>
+      </c>
       <c r="C298" s="3"/>
-      <c r="D298" s="12"/>
-    </row>
-    <row r="299" spans="1:4">
+      <c r="D298" s="12" t="s">
+        <v>766</v>
+      </c>
+      <c r="E298" s="17" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="299" spans="1:5">
       <c r="A299" s="18">
         <v>298</v>
       </c>
@@ -8649,7 +9042,7 @@
       <c r="C299" s="3"/>
       <c r="D299" s="12"/>
     </row>
-    <row r="300" spans="1:4">
+    <row r="300" spans="1:5">
       <c r="A300" s="18">
         <v>299</v>
       </c>
@@ -8657,7 +9050,7 @@
       <c r="C300" s="3"/>
       <c r="D300" s="12"/>
     </row>
-    <row r="301" spans="1:4">
+    <row r="301" spans="1:5">
       <c r="A301" s="18">
         <v>300</v>
       </c>
@@ -8665,7 +9058,7 @@
       <c r="C301" s="3"/>
       <c r="D301" s="12"/>
     </row>
-    <row r="302" spans="1:4">
+    <row r="302" spans="1:5">
       <c r="A302" s="18">
         <v>301</v>
       </c>
@@ -8673,7 +9066,7 @@
       <c r="C302" s="3"/>
       <c r="D302" s="12"/>
     </row>
-    <row r="303" spans="1:4">
+    <row r="303" spans="1:5">
       <c r="A303" s="18">
         <v>302</v>
       </c>
@@ -8681,7 +9074,7 @@
       <c r="C303" s="3"/>
       <c r="D303" s="12"/>
     </row>
-    <row r="304" spans="1:4">
+    <row r="304" spans="1:5">
       <c r="A304" s="18">
         <v>303</v>
       </c>

</xml_diff>

<commit_message>
add new posts 2023-09
</commit_message>
<xml_diff>
--- a/source/_posts/collection/new-words.xlsx
+++ b/source/_posts/collection/new-words.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/liuxiyang/myData/python-project/liuxiyang641.github.io/source/_posts/collection/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C494C47C-AC1A-B94F-BF08-DFEE2D43F310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B88E4903-E5F7-234D-84CF-702F54759335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-33600" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{C07A63B5-5344-AF4A-AFD6-2139CC657E22}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="783" uniqueCount="768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="780">
   <si>
     <t>[rɪˈtriːvl]</t>
   </si>
@@ -4515,6 +4515,140 @@
         <family val="1"/>
       </rPr>
       <t xml:space="preserve"> a NER model from learning such patterns effectively</t>
+    </r>
+  </si>
+  <si>
+    <t>performant</t>
+  </si>
+  <si>
+    <t>高效的，有效的</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We perform error analysis across </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>performant</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>nonperformant</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> prompts.</t>
+    </r>
+  </si>
+  <si>
+    <t>ingredient</t>
+  </si>
+  <si>
+    <t>因素，要素</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Another key </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>ingredient</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> for this revolution was the MS MARCO dataset.</t>
+    </r>
+  </si>
+  <si>
+    <t>practitioners</t>
+  </si>
+  <si>
+    <t>从业人员</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To circumvent these deployment challenges of large models, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>practitioners</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> often choose to deploy smaller specialized models instead.</t>
+    </r>
+  </si>
+  <si>
+    <t>circumvent</t>
+  </si>
+  <si>
+    <t>规避，绕过，逃避</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>circumvent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> these deployment challenges of large models, practitioners often choose to deploy smaller specialized models instead.</t>
     </r>
   </si>
 </sst>
@@ -5003,8 +5137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03B4733E-376B-124B-AFDB-49936A421CEF}">
   <dimension ref="A1:H696"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A294" zoomScale="125" workbookViewId="0">
-      <selection activeCell="I312" sqref="I312"/>
+    <sheetView tabSelected="1" topLeftCell="A297" zoomScale="125" workbookViewId="0">
+      <selection activeCell="H309" sqref="H309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -9034,37 +9168,65 @@
         <v>767</v>
       </c>
     </row>
-    <row r="299" spans="1:5">
+    <row r="299" spans="1:5" ht="38">
       <c r="A299" s="18">
         <v>298</v>
       </c>
-      <c r="B299" s="3"/>
+      <c r="B299" s="3" t="s">
+        <v>768</v>
+      </c>
       <c r="C299" s="3"/>
-      <c r="D299" s="12"/>
-    </row>
-    <row r="300" spans="1:5">
+      <c r="D299" s="12" t="s">
+        <v>769</v>
+      </c>
+      <c r="E299" s="17" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="300" spans="1:5" ht="38">
       <c r="A300" s="18">
         <v>299</v>
       </c>
-      <c r="B300" s="3"/>
+      <c r="B300" s="3" t="s">
+        <v>771</v>
+      </c>
       <c r="C300" s="3"/>
-      <c r="D300" s="12"/>
-    </row>
-    <row r="301" spans="1:5">
+      <c r="D300" s="12" t="s">
+        <v>772</v>
+      </c>
+      <c r="E300" s="17" t="s">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" ht="76">
       <c r="A301" s="18">
         <v>300</v>
       </c>
-      <c r="B301" s="3"/>
+      <c r="B301" s="3" t="s">
+        <v>774</v>
+      </c>
       <c r="C301" s="3"/>
-      <c r="D301" s="12"/>
-    </row>
-    <row r="302" spans="1:5">
+      <c r="D301" s="12" t="s">
+        <v>775</v>
+      </c>
+      <c r="E301" s="17" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" ht="76">
       <c r="A302" s="18">
         <v>301</v>
       </c>
-      <c r="B302" s="3"/>
+      <c r="B302" s="3" t="s">
+        <v>777</v>
+      </c>
       <c r="C302" s="3"/>
-      <c r="D302" s="12"/>
+      <c r="D302" s="12" t="s">
+        <v>778</v>
+      </c>
+      <c r="E302" s="17" t="s">
+        <v>779</v>
+      </c>
     </row>
     <row r="303" spans="1:5">
       <c r="A303" s="18">

</xml_diff>